<commit_message>
Remove all __pycache__ folders from repository
</commit_message>
<xml_diff>
--- a/design_docs/Settlement.xlsx
+++ b/design_docs/Settlement.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="81">
   <si>
     <t>id</t>
   </si>
@@ -113,6 +113,165 @@
   </si>
   <si>
     <t>所有葫芦（Full House）的牌型得分增加75%</t>
+  </si>
+  <si>
+    <t>Royal Flush</t>
+  </si>
+  <si>
+    <t>Straight Flush</t>
+  </si>
+  <si>
+    <t>Four of a Kind</t>
+  </si>
+  <si>
+    <t>Hulu</t>
+  </si>
+  <si>
+    <t>SAmehua</t>
+  </si>
+  <si>
+    <t>Flush</t>
+  </si>
+  <si>
+    <t>Three of a kind</t>
+  </si>
+  <si>
+    <t>Two Pairs</t>
+  </si>
+  <si>
+    <t>Pairs</t>
+  </si>
+  <si>
+    <t>High Card</t>
+  </si>
+  <si>
+    <t>HT</t>
+  </si>
+  <si>
+    <t>HJ</t>
+  </si>
+  <si>
+    <t>HQ</t>
+  </si>
+  <si>
+    <t>HK</t>
+  </si>
+  <si>
+    <t>HA</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>S4</t>
+  </si>
+  <si>
+    <t>S5</t>
+  </si>
+  <si>
+    <t>S6</t>
+  </si>
+  <si>
+    <t>S7</t>
+  </si>
+  <si>
+    <t>S8</t>
+  </si>
+  <si>
+    <t>S9</t>
+  </si>
+  <si>
+    <t>ST</t>
+  </si>
+  <si>
+    <t>SJ</t>
+  </si>
+  <si>
+    <t>SQ</t>
+  </si>
+  <si>
+    <t>SA</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>D5</t>
+  </si>
+  <si>
+    <t>D6</t>
+  </si>
+  <si>
+    <t>D7</t>
+  </si>
+  <si>
+    <t>D8</t>
+  </si>
+  <si>
+    <t>D9</t>
+  </si>
+  <si>
+    <t>DT</t>
+  </si>
+  <si>
+    <t>DJ</t>
+  </si>
+  <si>
+    <t>DQ</t>
+  </si>
+  <si>
+    <t>DK</t>
+  </si>
+  <si>
+    <t>DA</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
+    <t>C9</t>
+  </si>
+  <si>
+    <t>CT</t>
+  </si>
+  <si>
+    <t>CJ</t>
+  </si>
+  <si>
+    <t>CQ</t>
+  </si>
+  <si>
+    <t>CK</t>
+  </si>
+  <si>
+    <t>CA</t>
   </si>
 </sst>
 </file>
@@ -1043,10 +1202,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:U11"/>
+  <dimension ref="A1:U64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:G1"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.1"/>
@@ -1082,7 +1241,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>101</v>
+        <v>501</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1093,7 +1252,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3">
-        <v>102</v>
+        <v>502</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -1110,7 +1269,7 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4">
-        <v>103</v>
+        <v>503</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1127,7 +1286,7 @@
     </row>
     <row r="5" spans="1:21">
       <c r="A5">
-        <v>104</v>
+        <v>504</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -1147,7 +1306,7 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6">
-        <v>105</v>
+        <v>505</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -1164,7 +1323,7 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7">
-        <v>106</v>
+        <v>506</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -1178,7 +1337,7 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8">
-        <v>107</v>
+        <v>507</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -1195,7 +1354,7 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9">
-        <v>108</v>
+        <v>508</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -1212,7 +1371,7 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10">
-        <v>109</v>
+        <v>509</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -1229,7 +1388,7 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11">
-        <v>110</v>
+        <v>510</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -1242,6 +1401,802 @@
       </c>
       <c r="H11" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12">
+        <v>101</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12">
+        <v>200</v>
+      </c>
+      <c r="E12">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13">
+        <v>102</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13">
+        <v>100</v>
+      </c>
+      <c r="E13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14">
+        <v>103</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14">
+        <v>60</v>
+      </c>
+      <c r="E14">
+        <v>7</v>
+      </c>
+      <c r="H14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15">
+        <v>104</v>
+      </c>
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15">
+        <v>40</v>
+      </c>
+      <c r="E15">
+        <v>4</v>
+      </c>
+      <c r="H15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16">
+        <v>105</v>
+      </c>
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16">
+        <v>35</v>
+      </c>
+      <c r="E16">
+        <v>4</v>
+      </c>
+      <c r="H16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17">
+        <v>106</v>
+      </c>
+      <c r="B17">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17">
+        <v>30</v>
+      </c>
+      <c r="E17">
+        <v>4</v>
+      </c>
+      <c r="H17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18">
+        <v>107</v>
+      </c>
+      <c r="B18">
+        <v>7</v>
+      </c>
+      <c r="C18" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18">
+        <v>30</v>
+      </c>
+      <c r="E18">
+        <v>3</v>
+      </c>
+      <c r="H18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19">
+        <v>108</v>
+      </c>
+      <c r="B19">
+        <v>8</v>
+      </c>
+      <c r="C19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19">
+        <v>20</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+      <c r="H19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20">
+        <v>109</v>
+      </c>
+      <c r="B20">
+        <v>9</v>
+      </c>
+      <c r="C20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20">
+        <v>10</v>
+      </c>
+      <c r="E20">
+        <v>2</v>
+      </c>
+      <c r="H20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21">
+        <v>110</v>
+      </c>
+      <c r="B21">
+        <v>10</v>
+      </c>
+      <c r="C21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21">
+        <v>5</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="H21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22">
+        <v>211</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23">
+        <v>212</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24">
+        <v>213</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25">
+        <v>214</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25" t="s">
+        <v>41</v>
+      </c>
+      <c r="D25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26">
+        <v>215</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27">
+        <v>216</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27" t="s">
+        <v>43</v>
+      </c>
+      <c r="D27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28">
+        <v>217</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28" t="s">
+        <v>44</v>
+      </c>
+      <c r="D28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29">
+        <v>218</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29" t="s">
+        <v>45</v>
+      </c>
+      <c r="D29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30">
+        <v>219</v>
+      </c>
+      <c r="B30">
+        <v>2</v>
+      </c>
+      <c r="C30" t="s">
+        <v>46</v>
+      </c>
+      <c r="D30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31">
+        <v>220</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31" t="s">
+        <v>47</v>
+      </c>
+      <c r="D31">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32">
+        <v>221</v>
+      </c>
+      <c r="B32">
+        <v>2</v>
+      </c>
+      <c r="C32" t="s">
+        <v>48</v>
+      </c>
+      <c r="D32">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33">
+        <v>222</v>
+      </c>
+      <c r="B33">
+        <v>2</v>
+      </c>
+      <c r="C33" t="s">
+        <v>49</v>
+      </c>
+      <c r="D33">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34">
+        <v>223</v>
+      </c>
+      <c r="B34">
+        <v>2</v>
+      </c>
+      <c r="C34" t="s">
+        <v>50</v>
+      </c>
+      <c r="D34">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35">
+        <v>224</v>
+      </c>
+      <c r="B35">
+        <v>2</v>
+      </c>
+      <c r="C35" t="s">
+        <v>51</v>
+      </c>
+      <c r="D35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36">
+        <v>225</v>
+      </c>
+      <c r="B36">
+        <v>2</v>
+      </c>
+      <c r="C36" t="s">
+        <v>52</v>
+      </c>
+      <c r="D36">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37">
+        <v>226</v>
+      </c>
+      <c r="B37">
+        <v>2</v>
+      </c>
+      <c r="C37" t="s">
+        <v>53</v>
+      </c>
+      <c r="D37">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38">
+        <v>227</v>
+      </c>
+      <c r="B38">
+        <v>2</v>
+      </c>
+      <c r="C38" t="s">
+        <v>54</v>
+      </c>
+      <c r="D38">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39">
+        <v>228</v>
+      </c>
+      <c r="B39">
+        <v>2</v>
+      </c>
+      <c r="C39" t="s">
+        <v>55</v>
+      </c>
+      <c r="D39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40">
+        <v>229</v>
+      </c>
+      <c r="B40">
+        <v>2</v>
+      </c>
+      <c r="C40" t="s">
+        <v>56</v>
+      </c>
+      <c r="D40">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41">
+        <v>230</v>
+      </c>
+      <c r="B41">
+        <v>2</v>
+      </c>
+      <c r="C41" t="s">
+        <v>57</v>
+      </c>
+      <c r="D41">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42">
+        <v>231</v>
+      </c>
+      <c r="B42">
+        <v>2</v>
+      </c>
+      <c r="C42" t="s">
+        <v>58</v>
+      </c>
+      <c r="D42">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43">
+        <v>232</v>
+      </c>
+      <c r="B43">
+        <v>2</v>
+      </c>
+      <c r="C43" t="s">
+        <v>59</v>
+      </c>
+      <c r="D43">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44">
+        <v>233</v>
+      </c>
+      <c r="B44">
+        <v>2</v>
+      </c>
+      <c r="C44" t="s">
+        <v>60</v>
+      </c>
+      <c r="D44">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45">
+        <v>234</v>
+      </c>
+      <c r="B45">
+        <v>2</v>
+      </c>
+      <c r="C45" t="s">
+        <v>61</v>
+      </c>
+      <c r="D45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46">
+        <v>235</v>
+      </c>
+      <c r="B46">
+        <v>2</v>
+      </c>
+      <c r="C46" t="s">
+        <v>62</v>
+      </c>
+      <c r="D46">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47">
+        <v>236</v>
+      </c>
+      <c r="B47">
+        <v>2</v>
+      </c>
+      <c r="C47" t="s">
+        <v>63</v>
+      </c>
+      <c r="D47">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48">
+        <v>237</v>
+      </c>
+      <c r="B48">
+        <v>2</v>
+      </c>
+      <c r="C48" t="s">
+        <v>64</v>
+      </c>
+      <c r="D48">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49">
+        <v>238</v>
+      </c>
+      <c r="B49">
+        <v>2</v>
+      </c>
+      <c r="C49" t="s">
+        <v>65</v>
+      </c>
+      <c r="D49">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50">
+        <v>239</v>
+      </c>
+      <c r="B50">
+        <v>2</v>
+      </c>
+      <c r="C50" t="s">
+        <v>66</v>
+      </c>
+      <c r="D50">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51">
+        <v>240</v>
+      </c>
+      <c r="B51">
+        <v>2</v>
+      </c>
+      <c r="C51" t="s">
+        <v>67</v>
+      </c>
+      <c r="D51">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52">
+        <v>241</v>
+      </c>
+      <c r="B52">
+        <v>2</v>
+      </c>
+      <c r="C52" t="s">
+        <v>68</v>
+      </c>
+      <c r="D52">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53">
+        <v>242</v>
+      </c>
+      <c r="B53">
+        <v>2</v>
+      </c>
+      <c r="C53" t="s">
+        <v>69</v>
+      </c>
+      <c r="D53">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54">
+        <v>243</v>
+      </c>
+      <c r="B54">
+        <v>2</v>
+      </c>
+      <c r="C54" t="s">
+        <v>70</v>
+      </c>
+      <c r="D54">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55">
+        <v>244</v>
+      </c>
+      <c r="B55">
+        <v>2</v>
+      </c>
+      <c r="C55" t="s">
+        <v>71</v>
+      </c>
+      <c r="D55">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56">
+        <v>245</v>
+      </c>
+      <c r="B56">
+        <v>2</v>
+      </c>
+      <c r="C56" t="s">
+        <v>72</v>
+      </c>
+      <c r="D56">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57">
+        <v>246</v>
+      </c>
+      <c r="B57">
+        <v>2</v>
+      </c>
+      <c r="C57" t="s">
+        <v>73</v>
+      </c>
+      <c r="D57">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58">
+        <v>247</v>
+      </c>
+      <c r="B58">
+        <v>2</v>
+      </c>
+      <c r="C58" t="s">
+        <v>74</v>
+      </c>
+      <c r="D58">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59">
+        <v>248</v>
+      </c>
+      <c r="B59">
+        <v>2</v>
+      </c>
+      <c r="C59" t="s">
+        <v>75</v>
+      </c>
+      <c r="D59">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60">
+        <v>249</v>
+      </c>
+      <c r="B60">
+        <v>2</v>
+      </c>
+      <c r="C60" t="s">
+        <v>76</v>
+      </c>
+      <c r="D60">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61">
+        <v>250</v>
+      </c>
+      <c r="B61">
+        <v>2</v>
+      </c>
+      <c r="C61" t="s">
+        <v>77</v>
+      </c>
+      <c r="D61">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62">
+        <v>251</v>
+      </c>
+      <c r="B62">
+        <v>2</v>
+      </c>
+      <c r="C62" t="s">
+        <v>78</v>
+      </c>
+      <c r="D62">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63">
+        <v>252</v>
+      </c>
+      <c r="B63">
+        <v>2</v>
+      </c>
+      <c r="C63" t="s">
+        <v>79</v>
+      </c>
+      <c r="D63">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64">
+        <v>253</v>
+      </c>
+      <c r="B64">
+        <v>2</v>
+      </c>
+      <c r="C64" t="s">
+        <v>80</v>
+      </c>
+      <c r="D64">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>